<commit_message>
Correction made to the India section
</commit_message>
<xml_diff>
--- a/ULT Centres - Events and Classes.xlsx
+++ b/ULT Centres - Events and Classes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>United Lodge of Theosophists Centres</t>
   </si>
@@ -370,38 +370,6 @@
     <t>All locations in India</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3" tint="0.39997558519241921"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Schedule</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of classes/events/meetings/talks are </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3" tint="0.39997558519241921"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not available</t>
-    </r>
-  </si>
-  <si>
     <t>All locations in Europe</t>
   </si>
   <si>
@@ -438,38 +406,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3" tint="0.39997558519241921"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Schedule</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of classes/events/meetings/talks are</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3" tint="0.39997558519241921"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> not available</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Lectures 2021: Lectures are available till May 2021 via Zoom. Recorded lectures are available on Youtube as well. </t>
     </r>
     <r>
@@ -574,6 +510,199 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Conferences and Meetings: held on the first Monday of every month. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Updated schedule not available</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conferences: monthly conferences held on the first Sunday of every month. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Schedule available
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Special Meetings: A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>schedule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> exists for special meetings but is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not updated</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Meetings: Held online on Wednesdays (15:30) and Saturdays (17:00). </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Schedule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of meetings, information on news and events </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>available</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> only via</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> post and/or email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> upon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> registration</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Schedule </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">of classes/events/meetings/talks are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not available</t>
+    </r>
+  </si>
+  <si>
+    <t>Free public lectures till June 2021
+Study class every Friday</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Conferences: monthly conferences held on the second Saturdays of every month. </t>
     </r>
     <r>
@@ -616,7 +745,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>held on the first Monday of every month</t>
+      <t>held on the first Monday of every month. Schedule available as PDFs</t>
     </r>
   </si>
   <si>
@@ -693,22 +822,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>year not indicated. Schedule available</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Conferences and Meetings: held on the first Monday of every month. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Updated schedule not available</t>
+      <t>year not indicated. Schedule available as PDFs</t>
     </r>
   </si>
   <si>
@@ -744,181 +858,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Schedule available</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Conferences: monthly conferences held on the first Sunday of every month. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Schedule available
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Special Meetings: A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>schedule</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> exists for special meetings but is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not updated</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Meetings: Held online on Wednesdays (15:30) and Saturdays (17:00). </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Schedule</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of meetings, information on news and events </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>available</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> only via</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> post and/or email</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> upon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> registration</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Schedule </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">of classes/events/meetings/talks are </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not available</t>
+      <t>Schedule available
+Study Meetings: Schedule available as PDFs</t>
     </r>
   </si>
 </sst>
@@ -1429,7 +1370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1461,6 +1402,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1470,127 +1513,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1896,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,11 +1852,11 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1925,188 +1869,188 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="2:8" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="49" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
     </row>
     <row r="6" spans="2:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="47"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="47"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
-      <c r="C11" s="47"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>8</v>
       </c>
-      <c r="C12" s="47"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>9</v>
       </c>
-      <c r="C13" s="47"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>10</v>
       </c>
-      <c r="C14" s="47"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>11</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>12</v>
       </c>
-      <c r="C16" s="47"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="33"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+    </row>
+    <row r="17" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>1</v>
       </c>
@@ -2116,14 +2060,14 @@
       <c r="D17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>2</v>
       </c>
@@ -2131,198 +2075,212 @@
       <c r="D18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18"/>
+      <c r="E18" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="51" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
+      <c r="E19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="2:8" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="52"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
+      <c r="E20" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
     </row>
     <row r="21" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C21" s="52"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="18"/>
+      <c r="E21" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>4</v>
       </c>
-      <c r="C22" s="52"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="35"/>
+      <c r="E22" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>5</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="35"/>
-    </row>
-    <row r="24" spans="2:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="51"/>
+      <c r="D23" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="2:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>6</v>
       </c>
-      <c r="C24" s="52"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="35"/>
+      <c r="E24" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="52"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35"/>
+      <c r="E25" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" spans="2:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>8</v>
       </c>
-      <c r="C26" s="52"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
+      <c r="E26" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>10</v>
       </c>
-      <c r="C27" s="52"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="18"/>
+      <c r="E27" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="2:8" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="C28" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="38"/>
+      <c r="E28" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="23"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="41"/>
+      <c r="D30" s="55"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="43"/>
+      <c r="D31" s="53"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="50"/>
+      <c r="D32" s="14"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="54"/>
+      <c r="C33" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="16"/>
     </row>
     <row r="34" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="45"/>
+      <c r="C34" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C5:C16"/>
+    <mergeCell ref="C19:C27"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E5:H5"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
@@ -2339,20 +2297,6 @@
     <mergeCell ref="E12:H16"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C5:C16"/>
-    <mergeCell ref="C19:C27"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>